<commit_message>
KH School 최종본 베타.
</commit_message>
<xml_diff>
--- a/kh db.xlsx
+++ b/kh db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17235" windowHeight="3555" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17235" windowHeight="3750"/>
   </bookViews>
   <sheets>
     <sheet name="회원관련 테이블" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="도서관련 테이블" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:S21"/>
+  <oleSize ref="A10:N18"/>
 </workbook>
 </file>
 
@@ -1193,7 +1193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -1639,7 +1639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>

</xml_diff>